<commit_message>
Updated Excel with bug list
</commit_message>
<xml_diff>
--- a/componentError.xlsx
+++ b/componentError.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Search dropdown" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Click  outside Document to remove dropdown</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Size Selection</t>
+  </si>
+  <si>
+    <t>Remove timestamp from selected value (Selected value should be in following formatDD/MM/YYY)</t>
   </si>
 </sst>
 </file>
@@ -430,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -457,9 +460,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1">
-        <v>3</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="B3" s="1"/>
     </row>
   </sheetData>
@@ -469,24 +470,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1">
+      <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
+      <c r="B1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -494,7 +495,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -502,19 +503,27 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -606,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>